<commit_message>
completed cleaning of NEON and EIDC data
</commit_message>
<xml_diff>
--- a/Data/Metadata/EIDC_metadata/Conwy/Metadata_Analytical methods_conwy catchment spatial water chemistry.xlsx
+++ b/Data/Metadata/EIDC_metadata/Conwy/Metadata_Analytical methods_conwy catchment spatial water chemistry.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwy-my.sharepoint.com/personal/lrock1_uwyo_edu/Documents/PhD_code/STOICH_Aim1/Data/Metadata/EIDC_metadata/Conwy/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_5ECAA4EFDBD2F01F699EEECC62093E1DD1F91BAF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="210" yWindow="4185" windowWidth="18780" windowHeight="8070"/>
+    <workbookView minimized="1" xWindow="4695" yWindow="3795" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analytical methods" sheetId="1" r:id="rId1"/>
@@ -802,8 +808,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1431,6 +1437,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1477,7 +1491,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1509,9 +1523,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1543,6 +1575,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1718,14 +1768,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="N30" sqref="N30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="2" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" style="6" customWidth="1"/>
@@ -1747,7 +1797,7 @@
     <col min="20" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="15" customFormat="1">
+    <row r="1" spans="1:19" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -1806,7 +1856,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>48</v>
       </c>
@@ -1853,7 +1903,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>78</v>
       </c>
@@ -1898,7 +1948,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>43</v>
       </c>
@@ -1949,7 +1999,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>43</v>
       </c>
@@ -1997,7 +2047,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>89</v>
       </c>
@@ -2044,7 +2094,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>100</v>
       </c>
@@ -2091,7 +2141,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>97</v>
       </c>
@@ -2138,7 +2188,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>77</v>
       </c>
@@ -2185,7 +2235,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>70</v>
       </c>
@@ -2232,7 +2282,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -2279,7 +2329,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>94</v>
       </c>
@@ -2326,7 +2376,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>103</v>
       </c>
@@ -2373,7 +2423,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
@@ -2420,7 +2470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>85</v>
       </c>
@@ -2467,7 +2517,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>57</v>
       </c>
@@ -2509,7 +2559,7 @@
       </c>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>81</v>
       </c>
@@ -2556,7 +2606,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>96</v>
       </c>
@@ -2603,7 +2653,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>87</v>
       </c>
@@ -2650,7 +2700,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
@@ -2700,7 +2750,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>68</v>
       </c>
@@ -2747,7 +2797,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>62</v>
       </c>
@@ -2794,7 +2844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>83</v>
       </c>
@@ -2840,7 +2890,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>16</v>
       </c>
@@ -2887,7 +2937,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:19">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>102</v>
       </c>
@@ -2934,7 +2984,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>74</v>
       </c>
@@ -2981,7 +3031,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>14</v>
       </c>
@@ -3028,7 +3078,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>82</v>
       </c>
@@ -3075,7 +3125,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>93</v>
       </c>
@@ -3122,7 +3172,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>15</v>
       </c>
@@ -3169,7 +3219,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>27</v>
       </c>
@@ -3222,7 +3272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>84</v>
       </c>
@@ -3270,7 +3320,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>86</v>
       </c>
@@ -3315,7 +3365,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>30</v>
       </c>
@@ -3368,7 +3418,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>23</v>
       </c>
@@ -3422,7 +3472,7 @@
       </c>
       <c r="S35" s="8"/>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>23</v>
       </c>
@@ -3476,7 +3526,7 @@
       </c>
       <c r="S36" s="8"/>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>23</v>
       </c>
@@ -3530,7 +3580,7 @@
       </c>
       <c r="S37" s="8"/>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>98</v>
       </c>
@@ -3577,7 +3627,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>38</v>
       </c>
@@ -3625,7 +3675,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>56</v>
       </c>
@@ -3668,7 +3718,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>257</v>
       </c>
@@ -3713,7 +3763,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>63</v>
       </c>
@@ -3747,7 +3797,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>104</v>
       </c>
@@ -3794,7 +3844,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>91</v>
       </c>
@@ -3841,7 +3891,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>101</v>
       </c>
@@ -3888,7 +3938,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>67</v>
       </c>
@@ -3924,7 +3974,7 @@
       <c r="Q46" s="4"/>
       <c r="R46" s="4"/>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>95</v>
       </c>
@@ -3972,7 +4022,7 @@
       </c>
       <c r="R47" s="4"/>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>79</v>
       </c>
@@ -4020,7 +4070,7 @@
       </c>
       <c r="R48" s="4"/>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>90</v>
       </c>
@@ -4068,7 +4118,7 @@
       </c>
       <c r="R49" s="4"/>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>61</v>
       </c>
@@ -4116,7 +4166,7 @@
       </c>
       <c r="R50" s="4"/>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>107</v>
       </c>
@@ -4164,7 +4214,7 @@
       </c>
       <c r="R51" s="4"/>
     </row>
-    <row r="52" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>17</v>
       </c>
@@ -4212,7 +4262,7 @@
       </c>
       <c r="R52" s="4"/>
     </row>
-    <row r="53" spans="1:19">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>92</v>
       </c>
@@ -4260,7 +4310,7 @@
       </c>
       <c r="R53" s="4"/>
     </row>
-    <row r="54" spans="1:19" s="4" customFormat="1">
+    <row r="54" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
         <v>72</v>
       </c>
@@ -4303,7 +4353,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="55" spans="1:19">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>106</v>
       </c>
@@ -4351,7 +4401,7 @@
       </c>
       <c r="R55" s="4"/>
     </row>
-    <row r="56" spans="1:19">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -4396,7 +4446,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="57" spans="1:19">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>50</v>
       </c>
@@ -4441,7 +4491,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="58" spans="1:19">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>99</v>
       </c>
@@ -4488,7 +4538,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="59" spans="1:19">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>80</v>
       </c>
@@ -4535,7 +4585,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>105</v>
       </c>
@@ -4582,7 +4632,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>88</v>
       </c>
@@ -4631,188 +4681,188 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1"/>
-    <hyperlink ref="C61" r:id="rId2"/>
-    <hyperlink ref="E4" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
-    <hyperlink ref="E18" r:id="rId5"/>
-    <hyperlink ref="C9" r:id="rId6"/>
-    <hyperlink ref="C4" r:id="rId7"/>
-    <hyperlink ref="C5" r:id="rId8"/>
-    <hyperlink ref="C6" r:id="rId9"/>
-    <hyperlink ref="C7" r:id="rId10"/>
-    <hyperlink ref="C8" r:id="rId11"/>
-    <hyperlink ref="C10" r:id="rId12"/>
-    <hyperlink ref="C12" r:id="rId13"/>
-    <hyperlink ref="C13" r:id="rId14"/>
-    <hyperlink ref="C14" r:id="rId15"/>
-    <hyperlink ref="C15" r:id="rId16"/>
-    <hyperlink ref="C16" r:id="rId17"/>
-    <hyperlink ref="C17" r:id="rId18"/>
-    <hyperlink ref="C18" r:id="rId19"/>
-    <hyperlink ref="C19" r:id="rId20"/>
-    <hyperlink ref="C20" r:id="rId21"/>
-    <hyperlink ref="C21" r:id="rId22"/>
-    <hyperlink ref="C24" r:id="rId23"/>
-    <hyperlink ref="C25" r:id="rId24"/>
-    <hyperlink ref="C26" r:id="rId25"/>
-    <hyperlink ref="C27" r:id="rId26"/>
-    <hyperlink ref="C28" r:id="rId27"/>
-    <hyperlink ref="C29" r:id="rId28"/>
-    <hyperlink ref="C30" r:id="rId29"/>
-    <hyperlink ref="C31" r:id="rId30"/>
-    <hyperlink ref="C32" r:id="rId31"/>
-    <hyperlink ref="C33" r:id="rId32"/>
-    <hyperlink ref="C34" r:id="rId33"/>
-    <hyperlink ref="C35" r:id="rId34"/>
-    <hyperlink ref="C36" r:id="rId35"/>
-    <hyperlink ref="C37" r:id="rId36"/>
-    <hyperlink ref="C38" r:id="rId37"/>
-    <hyperlink ref="C39" r:id="rId38"/>
-    <hyperlink ref="C43" r:id="rId39"/>
-    <hyperlink ref="C44" r:id="rId40"/>
-    <hyperlink ref="C45" r:id="rId41"/>
-    <hyperlink ref="C47" r:id="rId42"/>
-    <hyperlink ref="C48" r:id="rId43"/>
-    <hyperlink ref="C49" r:id="rId44"/>
-    <hyperlink ref="C50" r:id="rId45"/>
-    <hyperlink ref="C51" r:id="rId46"/>
-    <hyperlink ref="C52" r:id="rId47"/>
-    <hyperlink ref="C53" r:id="rId48"/>
-    <hyperlink ref="C54" r:id="rId49"/>
-    <hyperlink ref="C55" r:id="rId50"/>
-    <hyperlink ref="C56" r:id="rId51"/>
-    <hyperlink ref="C57" r:id="rId52"/>
-    <hyperlink ref="C58" r:id="rId53"/>
-    <hyperlink ref="C59" r:id="rId54"/>
-    <hyperlink ref="C60" r:id="rId55"/>
-    <hyperlink ref="E5" r:id="rId56"/>
-    <hyperlink ref="E6" r:id="rId57"/>
-    <hyperlink ref="E7" r:id="rId58"/>
-    <hyperlink ref="E8" r:id="rId59"/>
-    <hyperlink ref="E10" r:id="rId60"/>
-    <hyperlink ref="E12" r:id="rId61"/>
-    <hyperlink ref="E13" r:id="rId62"/>
-    <hyperlink ref="E15" r:id="rId63"/>
-    <hyperlink ref="E16" r:id="rId64"/>
-    <hyperlink ref="E17" r:id="rId65"/>
-    <hyperlink ref="E19" r:id="rId66"/>
-    <hyperlink ref="E20" r:id="rId67"/>
-    <hyperlink ref="E21" r:id="rId68"/>
-    <hyperlink ref="E25" r:id="rId69"/>
-    <hyperlink ref="E26" r:id="rId70"/>
-    <hyperlink ref="E28" r:id="rId71"/>
-    <hyperlink ref="E32" r:id="rId72"/>
-    <hyperlink ref="E36" r:id="rId73"/>
-    <hyperlink ref="E37" r:id="rId74"/>
-    <hyperlink ref="E38" r:id="rId75"/>
-    <hyperlink ref="E40" r:id="rId76"/>
-    <hyperlink ref="E41" r:id="rId77"/>
-    <hyperlink ref="E43" r:id="rId78"/>
-    <hyperlink ref="E45" r:id="rId79"/>
-    <hyperlink ref="E47" r:id="rId80"/>
-    <hyperlink ref="E48" r:id="rId81"/>
-    <hyperlink ref="E49" r:id="rId82"/>
-    <hyperlink ref="E51" r:id="rId83"/>
-    <hyperlink ref="E50" r:id="rId84"/>
-    <hyperlink ref="E53" r:id="rId85"/>
-    <hyperlink ref="E54" r:id="rId86"/>
-    <hyperlink ref="E55" r:id="rId87"/>
-    <hyperlink ref="E56" r:id="rId88"/>
-    <hyperlink ref="E57" r:id="rId89"/>
-    <hyperlink ref="E59" r:id="rId90"/>
-    <hyperlink ref="E61" r:id="rId91"/>
-    <hyperlink ref="E58" r:id="rId92"/>
-    <hyperlink ref="E60" r:id="rId93"/>
-    <hyperlink ref="E42" r:id="rId94"/>
-    <hyperlink ref="E34" r:id="rId95"/>
-    <hyperlink ref="E35" r:id="rId96"/>
-    <hyperlink ref="E46" r:id="rId97"/>
-    <hyperlink ref="O40" r:id="rId98"/>
-    <hyperlink ref="Q40" r:id="rId99"/>
-    <hyperlink ref="C41" r:id="rId100"/>
-    <hyperlink ref="C22" r:id="rId101"/>
-    <hyperlink ref="K2" r:id="rId102"/>
-    <hyperlink ref="M2" r:id="rId103"/>
-    <hyperlink ref="K4" r:id="rId104"/>
-    <hyperlink ref="K5" r:id="rId105"/>
-    <hyperlink ref="K39" r:id="rId106"/>
-    <hyperlink ref="K16" r:id="rId107"/>
-    <hyperlink ref="K46" r:id="rId108"/>
-    <hyperlink ref="K41" r:id="rId109"/>
-    <hyperlink ref="O22" r:id="rId110"/>
-    <hyperlink ref="M3" r:id="rId111"/>
-    <hyperlink ref="M4" r:id="rId112"/>
-    <hyperlink ref="M5" r:id="rId113"/>
-    <hyperlink ref="M6" r:id="rId114"/>
-    <hyperlink ref="M8" r:id="rId115"/>
-    <hyperlink ref="M9" r:id="rId116"/>
-    <hyperlink ref="M10" r:id="rId117"/>
-    <hyperlink ref="M12" r:id="rId118"/>
-    <hyperlink ref="M13" r:id="rId119"/>
-    <hyperlink ref="M14" r:id="rId120"/>
-    <hyperlink ref="M15" r:id="rId121"/>
-    <hyperlink ref="M16" r:id="rId122"/>
-    <hyperlink ref="M17" r:id="rId123"/>
-    <hyperlink ref="M18" r:id="rId124"/>
-    <hyperlink ref="M19" r:id="rId125"/>
-    <hyperlink ref="M20" r:id="rId126"/>
-    <hyperlink ref="M21" r:id="rId127"/>
-    <hyperlink ref="M23" r:id="rId128"/>
-    <hyperlink ref="M25" r:id="rId129"/>
-    <hyperlink ref="M26" r:id="rId130"/>
-    <hyperlink ref="M28" r:id="rId131"/>
-    <hyperlink ref="M29" r:id="rId132"/>
-    <hyperlink ref="M31" r:id="rId133"/>
-    <hyperlink ref="M32" r:id="rId134"/>
-    <hyperlink ref="M33" r:id="rId135"/>
-    <hyperlink ref="M34" r:id="rId136"/>
-    <hyperlink ref="M35" r:id="rId137"/>
-    <hyperlink ref="M36" r:id="rId138"/>
-    <hyperlink ref="M37" r:id="rId139"/>
-    <hyperlink ref="M38" r:id="rId140"/>
-    <hyperlink ref="M39" r:id="rId141"/>
-    <hyperlink ref="M40" r:id="rId142"/>
-    <hyperlink ref="M41" r:id="rId143"/>
-    <hyperlink ref="M42" r:id="rId144"/>
-    <hyperlink ref="M43" r:id="rId145"/>
-    <hyperlink ref="M44" r:id="rId146"/>
-    <hyperlink ref="M46" r:id="rId147"/>
-    <hyperlink ref="M47" r:id="rId148"/>
-    <hyperlink ref="M48" r:id="rId149"/>
-    <hyperlink ref="M49" r:id="rId150"/>
-    <hyperlink ref="M51" r:id="rId151"/>
-    <hyperlink ref="M52" r:id="rId152"/>
-    <hyperlink ref="M53" r:id="rId153"/>
-    <hyperlink ref="M54" r:id="rId154"/>
-    <hyperlink ref="M55" r:id="rId155"/>
-    <hyperlink ref="M56" r:id="rId156"/>
-    <hyperlink ref="M57" r:id="rId157"/>
-    <hyperlink ref="M58" r:id="rId158"/>
-    <hyperlink ref="M59" r:id="rId159"/>
-    <hyperlink ref="M60" r:id="rId160"/>
-    <hyperlink ref="M61" r:id="rId161"/>
-    <hyperlink ref="O2" r:id="rId162"/>
-    <hyperlink ref="O4" r:id="rId163"/>
-    <hyperlink ref="O5" r:id="rId164"/>
-    <hyperlink ref="O6" r:id="rId165"/>
-    <hyperlink ref="O10" r:id="rId166"/>
-    <hyperlink ref="Q4" r:id="rId167"/>
-    <hyperlink ref="Q6" r:id="rId168"/>
-    <hyperlink ref="C3" r:id="rId169"/>
-    <hyperlink ref="E23" r:id="rId170"/>
-    <hyperlink ref="C23" r:id="rId171"/>
-    <hyperlink ref="E24" r:id="rId172"/>
-    <hyperlink ref="E27" r:id="rId173"/>
-    <hyperlink ref="E30" r:id="rId174"/>
-    <hyperlink ref="E14" r:id="rId175"/>
-    <hyperlink ref="E11" r:id="rId176"/>
-    <hyperlink ref="E22" r:id="rId177"/>
-    <hyperlink ref="E31" r:id="rId178"/>
-    <hyperlink ref="E2" r:id="rId179"/>
-    <hyperlink ref="E33" r:id="rId180"/>
-    <hyperlink ref="E52" r:id="rId181"/>
-    <hyperlink ref="C40" r:id="rId182"/>
+    <hyperlink ref="C11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C61" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E18" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="C6" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C7" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="C8" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="C10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="C12" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="C13" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="C14" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="C15" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C16" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="C17" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="C18" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="C19" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="C20" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="C21" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="C26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="C28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="C29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="C31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="C32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="C33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="C34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="C35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="C36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="C37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="C38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="C39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="C43" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="C44" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="C45" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="C47" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="C48" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="C49" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="C50" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="C51" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="C52" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="C53" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="C54" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="C55" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="C56" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="C57" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="C58" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="C59" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="C60" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="E5" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="E6" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="E7" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E8" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="E10" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="E12" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="E13" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="E15" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="E16" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="E17" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="E19" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="E20" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="E21" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="E25" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="E26" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="E28" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="E32" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="E36" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="E37" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="E38" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="E40" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="E41" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="E43" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="E45" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="E47" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="E48" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="E49" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="E51" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="E50" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="E53" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="E54" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="E55" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="E56" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="E57" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="E59" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="E61" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="E58" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="E60" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="E42" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="E34" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="E35" r:id="rId96" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="E46" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="O40" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="Q40" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="C41" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="C22" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="K2" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="M2" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="K4" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="K5" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="K39" r:id="rId106" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="K16" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="K46" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="K41" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="O22" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="M3" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="M4" r:id="rId112" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="M5" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="M6" r:id="rId114" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="M8" r:id="rId115" xr:uid="{00000000-0004-0000-0000-000072000000}"/>
+    <hyperlink ref="M9" r:id="rId116" xr:uid="{00000000-0004-0000-0000-000073000000}"/>
+    <hyperlink ref="M10" r:id="rId117" xr:uid="{00000000-0004-0000-0000-000074000000}"/>
+    <hyperlink ref="M12" r:id="rId118" xr:uid="{00000000-0004-0000-0000-000075000000}"/>
+    <hyperlink ref="M13" r:id="rId119" xr:uid="{00000000-0004-0000-0000-000076000000}"/>
+    <hyperlink ref="M14" r:id="rId120" xr:uid="{00000000-0004-0000-0000-000077000000}"/>
+    <hyperlink ref="M15" r:id="rId121" xr:uid="{00000000-0004-0000-0000-000078000000}"/>
+    <hyperlink ref="M16" r:id="rId122" xr:uid="{00000000-0004-0000-0000-000079000000}"/>
+    <hyperlink ref="M17" r:id="rId123" xr:uid="{00000000-0004-0000-0000-00007A000000}"/>
+    <hyperlink ref="M18" r:id="rId124" xr:uid="{00000000-0004-0000-0000-00007B000000}"/>
+    <hyperlink ref="M19" r:id="rId125" xr:uid="{00000000-0004-0000-0000-00007C000000}"/>
+    <hyperlink ref="M20" r:id="rId126" xr:uid="{00000000-0004-0000-0000-00007D000000}"/>
+    <hyperlink ref="M21" r:id="rId127" xr:uid="{00000000-0004-0000-0000-00007E000000}"/>
+    <hyperlink ref="M23" r:id="rId128" xr:uid="{00000000-0004-0000-0000-00007F000000}"/>
+    <hyperlink ref="M25" r:id="rId129" xr:uid="{00000000-0004-0000-0000-000080000000}"/>
+    <hyperlink ref="M26" r:id="rId130" xr:uid="{00000000-0004-0000-0000-000081000000}"/>
+    <hyperlink ref="M28" r:id="rId131" xr:uid="{00000000-0004-0000-0000-000082000000}"/>
+    <hyperlink ref="M29" r:id="rId132" xr:uid="{00000000-0004-0000-0000-000083000000}"/>
+    <hyperlink ref="M31" r:id="rId133" xr:uid="{00000000-0004-0000-0000-000084000000}"/>
+    <hyperlink ref="M32" r:id="rId134" xr:uid="{00000000-0004-0000-0000-000085000000}"/>
+    <hyperlink ref="M33" r:id="rId135" xr:uid="{00000000-0004-0000-0000-000086000000}"/>
+    <hyperlink ref="M34" r:id="rId136" xr:uid="{00000000-0004-0000-0000-000087000000}"/>
+    <hyperlink ref="M35" r:id="rId137" xr:uid="{00000000-0004-0000-0000-000088000000}"/>
+    <hyperlink ref="M36" r:id="rId138" xr:uid="{00000000-0004-0000-0000-000089000000}"/>
+    <hyperlink ref="M37" r:id="rId139" xr:uid="{00000000-0004-0000-0000-00008A000000}"/>
+    <hyperlink ref="M38" r:id="rId140" xr:uid="{00000000-0004-0000-0000-00008B000000}"/>
+    <hyperlink ref="M39" r:id="rId141" xr:uid="{00000000-0004-0000-0000-00008C000000}"/>
+    <hyperlink ref="M40" r:id="rId142" xr:uid="{00000000-0004-0000-0000-00008D000000}"/>
+    <hyperlink ref="M41" r:id="rId143" xr:uid="{00000000-0004-0000-0000-00008E000000}"/>
+    <hyperlink ref="M42" r:id="rId144" xr:uid="{00000000-0004-0000-0000-00008F000000}"/>
+    <hyperlink ref="M43" r:id="rId145" xr:uid="{00000000-0004-0000-0000-000090000000}"/>
+    <hyperlink ref="M44" r:id="rId146" xr:uid="{00000000-0004-0000-0000-000091000000}"/>
+    <hyperlink ref="M46" r:id="rId147" xr:uid="{00000000-0004-0000-0000-000092000000}"/>
+    <hyperlink ref="M47" r:id="rId148" xr:uid="{00000000-0004-0000-0000-000093000000}"/>
+    <hyperlink ref="M48" r:id="rId149" xr:uid="{00000000-0004-0000-0000-000094000000}"/>
+    <hyperlink ref="M49" r:id="rId150" xr:uid="{00000000-0004-0000-0000-000095000000}"/>
+    <hyperlink ref="M51" r:id="rId151" xr:uid="{00000000-0004-0000-0000-000096000000}"/>
+    <hyperlink ref="M52" r:id="rId152" xr:uid="{00000000-0004-0000-0000-000097000000}"/>
+    <hyperlink ref="M53" r:id="rId153" xr:uid="{00000000-0004-0000-0000-000098000000}"/>
+    <hyperlink ref="M54" r:id="rId154" xr:uid="{00000000-0004-0000-0000-000099000000}"/>
+    <hyperlink ref="M55" r:id="rId155" xr:uid="{00000000-0004-0000-0000-00009A000000}"/>
+    <hyperlink ref="M56" r:id="rId156" xr:uid="{00000000-0004-0000-0000-00009B000000}"/>
+    <hyperlink ref="M57" r:id="rId157" xr:uid="{00000000-0004-0000-0000-00009C000000}"/>
+    <hyperlink ref="M58" r:id="rId158" xr:uid="{00000000-0004-0000-0000-00009D000000}"/>
+    <hyperlink ref="M59" r:id="rId159" xr:uid="{00000000-0004-0000-0000-00009E000000}"/>
+    <hyperlink ref="M60" r:id="rId160" xr:uid="{00000000-0004-0000-0000-00009F000000}"/>
+    <hyperlink ref="M61" r:id="rId161" xr:uid="{00000000-0004-0000-0000-0000A0000000}"/>
+    <hyperlink ref="O2" r:id="rId162" xr:uid="{00000000-0004-0000-0000-0000A1000000}"/>
+    <hyperlink ref="O4" r:id="rId163" xr:uid="{00000000-0004-0000-0000-0000A2000000}"/>
+    <hyperlink ref="O5" r:id="rId164" xr:uid="{00000000-0004-0000-0000-0000A3000000}"/>
+    <hyperlink ref="O6" r:id="rId165" xr:uid="{00000000-0004-0000-0000-0000A4000000}"/>
+    <hyperlink ref="O10" r:id="rId166" xr:uid="{00000000-0004-0000-0000-0000A5000000}"/>
+    <hyperlink ref="Q4" r:id="rId167" xr:uid="{00000000-0004-0000-0000-0000A6000000}"/>
+    <hyperlink ref="Q6" r:id="rId168" xr:uid="{00000000-0004-0000-0000-0000A7000000}"/>
+    <hyperlink ref="C3" r:id="rId169" xr:uid="{00000000-0004-0000-0000-0000A8000000}"/>
+    <hyperlink ref="E23" r:id="rId170" xr:uid="{00000000-0004-0000-0000-0000A9000000}"/>
+    <hyperlink ref="C23" r:id="rId171" xr:uid="{00000000-0004-0000-0000-0000AA000000}"/>
+    <hyperlink ref="E24" r:id="rId172" xr:uid="{00000000-0004-0000-0000-0000AB000000}"/>
+    <hyperlink ref="E27" r:id="rId173" xr:uid="{00000000-0004-0000-0000-0000AC000000}"/>
+    <hyperlink ref="E30" r:id="rId174" xr:uid="{00000000-0004-0000-0000-0000AD000000}"/>
+    <hyperlink ref="E14" r:id="rId175" xr:uid="{00000000-0004-0000-0000-0000AE000000}"/>
+    <hyperlink ref="E11" r:id="rId176" xr:uid="{00000000-0004-0000-0000-0000AF000000}"/>
+    <hyperlink ref="E22" r:id="rId177" xr:uid="{00000000-0004-0000-0000-0000B0000000}"/>
+    <hyperlink ref="E31" r:id="rId178" xr:uid="{00000000-0004-0000-0000-0000B1000000}"/>
+    <hyperlink ref="E2" r:id="rId179" xr:uid="{00000000-0004-0000-0000-0000B2000000}"/>
+    <hyperlink ref="E33" r:id="rId180" xr:uid="{00000000-0004-0000-0000-0000B3000000}"/>
+    <hyperlink ref="E52" r:id="rId181" xr:uid="{00000000-0004-0000-0000-0000B4000000}"/>
+    <hyperlink ref="C40" r:id="rId182" xr:uid="{00000000-0004-0000-0000-0000B5000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId183"/>

</xml_diff>